<commit_message>
Implementation of HLD and LLD, Insertion of graphics, bank update
</commit_message>
<xml_diff>
--- a/Documentação/Backlog do projeto.xlsx
+++ b/Documentação/Backlog do projeto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Behavior\Desktop\Pantec\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1CCB48-17A7-4638-991C-1D0E65065F6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD33C905-2C00-4281-89A3-0EBA2810FD08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="210" windowWidth="15375" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="780" windowWidth="15375" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -69,9 +69,6 @@
     <t xml:space="preserve">O sistema deverá ter tela de login </t>
   </si>
   <si>
-    <t>A aplicação possuira graficos para administração de recursos da maquina</t>
-  </si>
-  <si>
     <t>Classificação</t>
   </si>
   <si>
@@ -127,13 +124,58 @@
   </si>
   <si>
     <t>O site devera ter uma tela para cadastro</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>O sistema deve ter um helpdesk</t>
+  </si>
+  <si>
+    <t>O sistema deverá utilizar a API OSHI p/ capitar os dados</t>
+  </si>
+  <si>
+    <t>A aplicação possuirá graficos para administração de recursos da maquina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +194,12 @@
       <color theme="1"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -503,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,18 +566,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>11</v>
@@ -540,7 +588,7 @@
     </row>
     <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -551,7 +599,7 @@
     </row>
     <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -562,7 +610,7 @@
     </row>
     <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -573,7 +621,7 @@
     </row>
     <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>6</v>
@@ -584,7 +632,7 @@
     </row>
     <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -595,7 +643,7 @@
     </row>
     <row r="8" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>8</v>
@@ -606,18 +654,18 @@
     </row>
     <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>9</v>
@@ -628,7 +676,7 @@
     </row>
     <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -639,7 +687,7 @@
     </row>
     <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>10</v>
@@ -650,10 +698,10 @@
     </row>
     <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
@@ -661,10 +709,10 @@
     </row>
     <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>1</v>
@@ -672,16 +720,109 @@
     </row>
     <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>